<commit_message>
Corretto errore test 4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1111MEDUSASOFTX/Medusa_Software/Urania_FSE/v.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1111MEDUSASOFTX/Medusa_Software/Urania_FSE/v.1.0.0/report-checklist.xlsx
@@ -574,13 +574,13 @@
     </r>
   </si>
   <si>
-    <t>2023-06-20T12:00:21Z</t>
-  </si>
-  <si>
-    <t>326f18c7379c2c0e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.edb6d60b7d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-07-01T21:00:12Z</t>
+  </si>
+  <si>
+    <t>e15d0e2169b5c1da</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.501f41cb88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -3907,7 +3907,7 @@
         <v>77</v>
       </c>
       <c r="F13" s="57">
-        <v>45097</v>
+        <v>45108</v>
       </c>
       <c r="G13" t="s" s="58">
         <v>78</v>

</xml_diff>